<commit_message>
Adding data for two scripts i different excel files
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,3269 +418,2639 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0677c559a31441ac51774383cc1e159081a6045453668d7f655d0fca46601364</v>
+        <v>12028327ff6744f6110c1d6fadd42f34a04d2d246b4142ea99615cabd51d2bb4</v>
       </c>
       <c r="B2">
-        <v>1742457968496</v>
+        <v>1742469357502</v>
       </c>
       <c r="C2">
-        <v>1742457969874</v>
+        <v>1742469358127</v>
       </c>
       <c r="D2">
-        <v>1378</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>77f821220860773ca467469253252a5afc80fa64d49abf0088ee555c0495ea78</v>
+        <v>35688d213033f07a528f6a74c69db9ffebe1c329cdbec82f3d89cc8da4d805ea</v>
       </c>
       <c r="B3">
-        <v>1742457968496</v>
+        <v>1742469357502</v>
       </c>
       <c r="C3">
-        <v>1742457969874</v>
+        <v>1742469358127</v>
       </c>
       <c r="D3">
-        <v>1378</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>d6f18cf3d6033dd8f36282097e482f623815006f79d20f2ee8f4b149adced6ac</v>
+        <v>5f5781adefaee7d7ba3f42c471c1139b00b5f50dcaea86638f24d668b3196066</v>
       </c>
       <c r="B4">
-        <v>1742457968496</v>
+        <v>1742469357502</v>
       </c>
       <c r="C4">
-        <v>1742457969874</v>
+        <v>1742469358128</v>
       </c>
       <c r="D4">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>cd31a4dd5d01cba138eb190e7d8cf2ba4d2474befaf43e5933b21fc0d3ff3c8c</v>
+        <v>208e2159c4cbe736fbf0710f3dd96421354c14f8125318bd052a17f90cec07d6</v>
       </c>
       <c r="B5">
-        <v>1742457968496</v>
+        <v>1742469357502</v>
       </c>
       <c r="C5">
-        <v>1742457969874</v>
+        <v>1742469358128</v>
       </c>
       <c r="D5">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>0bf7985661739693eb136947bb56bc834d170fa534beaf8c82b71a443c28d284</v>
+        <v>bfd8004d7e8f14a38090b6521f6736d3491fb8ad32e054f84e84d1dc50466197</v>
       </c>
       <c r="B6">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C6">
-        <v>1742457969875</v>
+        <v>1742469358128</v>
       </c>
       <c r="D6">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>661210b3a60fec6e96409186ff9f52fc51ade01240902b56acf03878c67ca20a</v>
+        <v>7b2ae5d17c58dde6c81359da0f8f770443cd85cacba6b93cf31a82d2a8dbd3f1</v>
       </c>
       <c r="B7">
-        <v>1742457968496</v>
+        <v>1742469357502</v>
       </c>
       <c r="C7">
-        <v>1742457969874</v>
+        <v>1742469358128</v>
       </c>
       <c r="D7">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>94ff251a6552addf579b1bb83ac31154fe2324186fcf540887f10710ba7c3bae</v>
+        <v>a1ad4008314ec9bd189bb1b729401ed894c8b77649fec956c0b0b0fd9849061b</v>
       </c>
       <c r="B8">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C8">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D8">
-        <v>1378</v>
+        <v>627</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>c067c823575e7d78bb3f16cb720c2eca64d43adbdff886cb61c5af832903ff5c</v>
+        <v>c94587717d912ce5c0678d816261ed9fc23789ace72b1e32d64323b506cd6495</v>
       </c>
       <c r="B9">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C9">
-        <v>1742457969875</v>
+        <v>1742469358128</v>
       </c>
       <c r="D9">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>3ff3dda7f8c9048b405935cc01cf15786b6fc056ca9540aaa706055746423ec0</v>
+        <v>d0e644209c4af680fbd3796f57f3471d2d20cf45b5f9e3d38ce3d82f15b06b8e</v>
       </c>
       <c r="B10">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C10">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D10">
-        <v>1378</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>8c197f179c6aa60548fc525088c74418eda2f86d45e1ef457972f2e4f6e65b7c</v>
+        <v>5cd8c55a8839680565d6a2a3001011aaae72a8f162cd3b5e81e74393b48e3665</v>
       </c>
       <c r="B11">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C11">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D11">
-        <v>1378</v>
+        <v>627</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>8c619ebd8e40ec5d2c3849bf904e3031cde184fe58946fddcf867ec720c975dd</v>
+        <v>9832c1ffeef759117e94b14aa9f946f47b05065e4c777a4ede8921d9a57d17eb</v>
       </c>
       <c r="B12">
-        <v>1742457968497</v>
+        <v>1742469357503</v>
       </c>
       <c r="C12">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D12">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>42b35885772d93794fbfc5b7f416e986c6d390d80c399eeb8adb33387236cb7a</v>
+        <v>bd3251ee0b83c37a5132921638baa996d20fd29273b3ddcaf39630de4776e8e6</v>
       </c>
       <c r="B13">
-        <v>1742457968497</v>
+        <v>1742469357502</v>
       </c>
       <c r="C13">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D13">
-        <v>1378</v>
+        <v>627</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>e0487bf7e93802b211d2f79a5cbd60513ef11318b37f26b99d942fd9414171e0</v>
+        <v>17af602a9c448ae8e26daf72114c1a71ecd5604dbcec2a42bd0bade608b84711</v>
       </c>
       <c r="B14">
-        <v>1742457968498</v>
+        <v>1742469357503</v>
       </c>
       <c r="C14">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D14">
-        <v>1377</v>
+        <v>626</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>ecd7e9f91ab72738493734071731495eaea4e0ed6894000e353b7ee617f2e772</v>
+        <v>36f4951b8ab144524dc09ec4f7679a557b0b8361dd9be341685a513619581b7b</v>
       </c>
       <c r="B15">
-        <v>1742457968497</v>
+        <v>1742469357503</v>
       </c>
       <c r="C15">
-        <v>1742457969875</v>
+        <v>1742469358129</v>
       </c>
       <c r="D15">
-        <v>1378</v>
+        <v>626</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>f40a606666ad02f30a2588527fb4e66274632b35375958892b232fa1f6e22d6e</v>
+        <v>295758dfe13eada8fc49771bcb46d2c11f2380d91ce3fcb2529ce3144b3054fa</v>
       </c>
       <c r="B16">
-        <v>1742457968497</v>
+        <v>1742469357503</v>
       </c>
       <c r="C16">
-        <v>1742457969875</v>
+        <v>1742469358130</v>
       </c>
       <c r="D16">
-        <v>1378</v>
+        <v>627</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>15d84a2a35adb8224a6150aca9498235a75afb09df45ce1f207fb29a4e03c17a</v>
+        <v>d9748e5941bbe1af1ac43a520c8a79738d05220d9b4eedcd5e203a76811661f0</v>
       </c>
       <c r="B17">
-        <v>1742457968498</v>
+        <v>1742469357503</v>
       </c>
       <c r="C17">
-        <v>1742457969875</v>
+        <v>1742469358130</v>
       </c>
       <c r="D17">
-        <v>1377</v>
+        <v>627</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>6f942cfef146201af28c269a2e3d0c24aa323f4efb5477942922230138848736</v>
+        <v>220f786d9969c0bf74915f6b9d694271ef28b0b8f02b8270a26faf3c9ecb4792</v>
       </c>
       <c r="B18">
-        <v>1742457968498</v>
+        <v>1742469357503</v>
       </c>
       <c r="C18">
-        <v>1742457969875</v>
+        <v>1742469358130</v>
       </c>
       <c r="D18">
-        <v>1377</v>
+        <v>627</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>eff4f4f73811672442908d270dd31b6c29f2b064647492ad246c3a736b4604f8</v>
+        <v>3aa2083330f0269f982292856598b46bcadda4b9562fec935b6a3af665bbeb35</v>
       </c>
       <c r="B19">
-        <v>1742457968498</v>
+        <v>1742469357503</v>
       </c>
       <c r="C19">
-        <v>1742457969875</v>
+        <v>1742469358130</v>
       </c>
       <c r="D19">
-        <v>1377</v>
+        <v>627</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>7c1b3c549d75c093622dc12d4f90baa9550b3a7d7ca4480060be2e2f56f307f0</v>
+        <v>bbcef62755b1ac29791f09679be066ee36880766ff0b1b52c715237725a3407b</v>
       </c>
       <c r="B20">
-        <v>1742457968498</v>
+        <v>1742469357503</v>
       </c>
       <c r="C20">
-        <v>1742457969875</v>
+        <v>1742469358130</v>
       </c>
       <c r="D20">
-        <v>1377</v>
+        <v>627</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>52cfb14626b372fb77ec5f0a59ae16eb0aecfed22c6886075957fabe3bfb0896</v>
+        <v>542a3c4aa80bdf36d5302db3898aaeccf84cb472e5cfd0ed8e926b7e77718c17</v>
       </c>
       <c r="B21">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C21">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D21">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>c34f148949ef0c2a969ca2ef0f5b7dfae817cc80df1b330ec01e9ee97ed761bc</v>
+        <v>1427828abbf00a7e9836796e99753c8e9fbf63763d0c3747648b0bbf4486912e</v>
       </c>
       <c r="B22">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C22">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D22">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>41ee5f19ecb35bcba11e8fc7e9be13c0faff93eed3ea462885c62ecdb6cf1950</v>
+        <v>f64df7ba05fffc2ec4cbedd6abfa84d4f437bae16c66c6fe6565d5c14a04ffe7</v>
       </c>
       <c r="B23">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C23">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D23">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>9a5befe983b6d1b030792046e653f8d51aeea41ece20d8440a7c2556b50b8e1c</v>
+        <v>79a8d01e073a2df84c48138aad32c6156e6610d6db83bf22d628fd022a00b8c0</v>
       </c>
       <c r="B24">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C24">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D24">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>516f72d6f3ca86dcbe69725e93437fb2019a748ee8cc06e99982c6c6cc7f784c</v>
+        <v>448cfcb48abb8f81d4cdbff7dcb0baf89b0c84bf82814375e68ca8c92c369c2f</v>
       </c>
       <c r="B25">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C25">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D25">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>7fe01bc4483ab775b3a9b69a4e47511d659ce5f6dead503959d94c1b26a627c7</v>
+        <v>6d1c255394c1505d0a89daa2479d0668241fb8b3b5b6c1e631bcb4d20fe9265d</v>
       </c>
       <c r="B26">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C26">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D26">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>0ab9fd7ad1b429129e598aeb5d5718274982fc5512bb7714602999609136c40b</v>
+        <v>7382150a34459aaa4c19ef8d3ce4430673f655c94b54c6768ed33c16b9c26211</v>
       </c>
       <c r="B27">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C27">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D27">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>a0180a15a17412ce1c14f7c9431ec1ac95fb9b9fc907f189756f087d3751d03e</v>
+        <v>c200364da42606e7c8448154bc3f18d02a8b2e405ee4895bc67128c238fe3eaf</v>
       </c>
       <c r="B28">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C28">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D28">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>71f8d9314571bd1affaa42e26937517177febb99da5b1d96a394ed904fa0e144</v>
+        <v>e6ff5237aa460ab3b100c36e75becaaddb7ab4571adaec90d5b6a791167cd6ab</v>
       </c>
       <c r="B29">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C29">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D29">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>f435e173de8121ce6d1631fcc2090137696873ee37a5d2f5facbc723eeeb4489</v>
+        <v>d5976763f6be834230ca7ed4881c65bcb57dc77fe550e3c17f7b06836a38930a</v>
       </c>
       <c r="B30">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C30">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D30">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>1ac69e080ecadb2e5fb7180277e895ed2dfa2cafd05e8c51c105423cbb919a9e</v>
+        <v>e0af504d7471d73320b9754699de5fa5e589f103ca8d24dea1a7a9559a10b10d</v>
       </c>
       <c r="B31">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C31">
-        <v>1742457970741</v>
+        <v>1742469358130</v>
       </c>
       <c r="D31">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>e8364788868e2353bdf816a7f242f64b917636862ad6effea4bce86554cbcdbc</v>
+        <v>3dbd18cb0b5467375befd2ad0f2677d9915bf3e20581261d9ea45d2ff172953f</v>
       </c>
       <c r="B32">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C32">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D32">
-        <v>2060</v>
+        <v>628</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>6306761bf747fa1df1648981b2e05a7031e6bfae196176cef2494938e38ef3fd</v>
+        <v>63b57d31aed5e688c0570ab3f12228130ffe216dabc983a73ad3ab39d4d55088</v>
       </c>
       <c r="B33">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C33">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D33">
-        <v>2060</v>
+        <v>628</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>da3275b85917cd793818648850d78dfb245ad4799c4324f66c25c3a6e3b96a5f</v>
+        <v>78ee17e1a35639c0907104a8e97901a237a235aab50ee54ba24e2ff1e020468c</v>
       </c>
       <c r="B34">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C34">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D34">
-        <v>2060</v>
+        <v>628</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>898c148d9b99ecd0053796acf341a8c3a319dbb2c67bd169685ebc976bd9fbf6</v>
+        <v>f63a645651d344d57102bf2d8542b6a0a6930609102c0a0f9423be3b3bbc3892</v>
       </c>
       <c r="B35">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C35">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D35">
-        <v>2061</v>
+        <v>628</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>af1524591f9ac836b901f1cd54b4e338d7fdbea66e54252597bd5d703b53ab7e</v>
+        <v>6bd9b354eea488405e863d84f65ecab7f5e92d1343972a107e2dca54f7cfb0d0</v>
       </c>
       <c r="B36">
-        <v>1742457968681</v>
+        <v>1742469357504</v>
       </c>
       <c r="C36">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D36">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>63c09f502ffffaf61c53d06f2e9b7f2d77c7098eab442d0019266aa5d90528df</v>
+        <v>5b33b4cd7bb76ce8b2061da9648ebb2112c16563f8e7787b233c7ae988e7426f</v>
       </c>
       <c r="B37">
-        <v>1742457968681</v>
+        <v>1742469357504</v>
       </c>
       <c r="C37">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D37">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>fb32eaf4f8b25a4899641203c0c81fe2099e85926866b45c702fff6adfb9e09f</v>
+        <v>b63863b773f62d46672e4a72ede50bbba02ab96da379e0f53e7f20f02987b0a7</v>
       </c>
       <c r="B38">
-        <v>1742457968681</v>
+        <v>1742469357503</v>
       </c>
       <c r="C38">
-        <v>1742457970741</v>
+        <v>1742469358131</v>
       </c>
       <c r="D38">
-        <v>2060</v>
+        <v>628</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>185dd8c0e99fe9825b687fe60a64a197fc7bf988ccacef0e5a205ee14a4e4132</v>
+        <v>7d4f328703920fc06a441ff78bedea89d6314a048daf4f8e199013fff6742f0a</v>
       </c>
       <c r="B39">
-        <v>1742457968682</v>
+        <v>1742469357504</v>
       </c>
       <c r="C39">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D39">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>8b5567fe1399f436341c7634c14d1e347b3260a0a5b0137ce0819fbc518b8ca4</v>
+        <v>eab39dfd7801fb8d24b3ef70f7c9a0d711bc6f8c7daebe48951ed997c5639c4f</v>
       </c>
       <c r="B40">
-        <v>1742457968681</v>
+        <v>1742469357505</v>
       </c>
       <c r="C40">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D40">
-        <v>2061</v>
+        <v>626</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>28d62a28ec2f5fc0655f515d331289f45f919f9f2252f5f3d443047036b6675d</v>
+        <v>59e6700bd1b94784fe96d738be98a87f3a323141d5f261fb49008af5643d10f5</v>
       </c>
       <c r="B41">
-        <v>1742457968681</v>
+        <v>1742469357505</v>
       </c>
       <c r="C41">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D41">
-        <v>2061</v>
+        <v>626</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>0f1f9932ec520d0d88c46189838c7b39ecd00da8def41960a03119b542bae20b</v>
+        <v>d0095804b08ede898d4a5139eda08e2b5f1cb316681e0d4af1738742d1ed1bd8</v>
       </c>
       <c r="B42">
-        <v>1742457968681</v>
+        <v>1742469357504</v>
       </c>
       <c r="C42">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D42">
-        <v>2061</v>
+        <v>627</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>175ac99c00fece0a0759f2e209c85b5183d1e583a96ea9f88c6223fe40c262b0</v>
+        <v>3cf0cc35e9d231ed09ebcff22e0caeb45a066c0891265b5149c67374a6a417f1</v>
       </c>
       <c r="B43">
-        <v>1742457968682</v>
+        <v>1742469357504</v>
       </c>
       <c r="C43">
-        <v>1742457970742</v>
+        <v>1742469358131</v>
       </c>
       <c r="D43">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>e56a06c0cd16e8fe74653350a6c12b92036f1562753d5fcefac1c2161d0c77f4</v>
+        <v>d1caa33603c8bcccf7e306ce2c50246b33199142ea4976f901d4d4dd4e53fea1</v>
       </c>
       <c r="B44">
-        <v>1742457968681</v>
+        <v>1742469357505</v>
       </c>
       <c r="C44">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D44">
-        <v>2061</v>
+        <v>627</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>97e85f9851ca328840017f9988f6eb7b6759a1ef1bb5f83e2a0b5e5abf83e239</v>
+        <v>0cd58c6ea0d0681e25b137d1bc66d1ab6b69886796e5902cca219a6874231301</v>
       </c>
       <c r="B45">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C45">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D45">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>85203c82d86fd676f30729e4438c22a39218511b99efe885c758fdd1f4cd1945</v>
+        <v>c4ff49d75855ff4ed3bea57d7223a1903ea6e68ee0def49378245a59057bc88f</v>
       </c>
       <c r="B46">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C46">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D46">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>702bb8581ecfe743b0c51e555696080d85879dc0a8f7187e078a635915cf3774</v>
+        <v>bc86df39e5171f3a6cc7a407a24a2c07d0b1036af95cce63074c189fea74b0e7</v>
       </c>
       <c r="B47">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C47">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D47">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>da689d9092314ca9e6f6c928aa14d27ca10f43fd6b0bf5c6ab41fe134d326dd4</v>
+        <v>bcfc6b9bd65d0f52054796d5ad0804bef49beaab1e83fff53bcadf3de301041b</v>
       </c>
       <c r="B48">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C48">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D48">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>278742895bd95b6c243d7445a049a71d60a1bc4087d34735d6692e17900dc584</v>
+        <v>d0ab690b478285622101802e9bec3a29920250f9cce2849be03d9977a1376e1a</v>
       </c>
       <c r="B49">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C49">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D49">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>00d1eb22fe5a2fa587579a960905b304f8029596aaa526ef7dd25ebf5a7d0d25</v>
+        <v>0aad63527f6e31444e9c695417e95883cfdee16cf06a2e14aabb957ffdab72fb</v>
       </c>
       <c r="B50">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C50">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D50">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>c979d82c1e154aa10ee869a22e76703712aeccfc26439ba2e35b4efdc895f346</v>
+        <v>ee99734854f424f8429b083adcf4318fa26fdb1629042f0a2d6e4679a7358b59</v>
       </c>
       <c r="B51">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C51">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D51">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>d2782747eb9fbefdce724b976517ba651f7114c4fc803a79450b1a3a5f0e4f0a</v>
+        <v>d02099fef10f2d5ef8468ff2eb42c4e26492d77fc05f9adedac335c9993406c1</v>
       </c>
       <c r="B52">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C52">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D52">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>47e1ce8813f96b6e20b8cb4c18601ac56fdc797acd068e0244820fbe1c35e719</v>
+        <v>217a417a0bb6481a602063c40cae9286826dc14bc64194dc4759f8abd9322878</v>
       </c>
       <c r="B53">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C53">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D53">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>bb7db0b0328ec082aa15c1a432312a4aaa70a6f45ae8fbe38113086f27a6ec06</v>
+        <v>57afaf17ec571de47984073c083a498a724d312c7e84fe40f79e9d5682580f0f</v>
       </c>
       <c r="B54">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C54">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D54">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>97d1c92363c740cfca27a959bc9879b8cf6118e889ba7663dde8cf682bb4e385</v>
+        <v>29c5d489b463d99853c31a42f50db2dcfaac4baa8145936fabcfe4a1a586c451</v>
       </c>
       <c r="B55">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C55">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D55">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>4b7400d2c3cdae8cefe6b182bae209ee24b9fd383334472353cf7c79fd6e62d4</v>
+        <v>db9af4b05443582078bd4be652323935ec0e6dcf3f6960ec3826e1d26cd3d0b3</v>
       </c>
       <c r="B56">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C56">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D56">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>7c5d441dc70272908296a994bca0c9bb8593dfff06d608acb1f0d99e22a71787</v>
+        <v>90a1baeb272f443219a4abd00668a4c087eda3a45549626208b1fc86c10550c9</v>
       </c>
       <c r="B57">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C57">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D57">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>7cd56701669c17c751554cad151182a332498e8a7c82fb4c7cf3f04cfe549acc</v>
+        <v>1d79c4592f526541059c4e23b220b5ffccff977542225f424c1195cfd6148b4f</v>
       </c>
       <c r="B58">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C58">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D58">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>486feba33a2ea2da1af64fd146df3474d4758589f1ea27991844537d42c0ac95</v>
+        <v>eb04c0d51746edc7a5f827041a03f253615356daceb469665c11962229721cee</v>
       </c>
       <c r="B59">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C59">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D59">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>dcf94e244caed87f81a7133bf8172882cfb1a2b5956c0c2579e00c185560caea</v>
+        <v>4e46d27ad3a985691e2a377157ebb48e99c43065da6ef7a76f14390fb6fe715b</v>
       </c>
       <c r="B60">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C60">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D60">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>56a3ef05403f3bf4f9deb556aae3e6da002474369836e09df12a9c8167fc4c4b</v>
+        <v>7473aac6d2e5585445ba3c90df9002523fc7efb5ce3327bc3c2692e87bf7b8d8</v>
       </c>
       <c r="B61">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C61">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D61">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>1967d80475654eff1356ea2c24673987de07a0f1095904e5bbf4839d03bd0a2c</v>
+        <v>b6ea380a2b3ceb75308d0c38f3f16c146d332207b3f7aeee870f96f94bf5350d</v>
       </c>
       <c r="B62">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C62">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D62">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>d1b321b3532935f10769218717cc678579f189595fcfb9075fe793b98b9e5464</v>
+        <v>3b26d72db511f4d698f4efccc2254479a3aaad3c351f093b53b1bf89ace8aa15</v>
       </c>
       <c r="B63">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C63">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D63">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>0cb496ce7d3c085be13054d21a53b5675f308a0e4b13cfbb20431d66ea1d05f5</v>
+        <v>4239f11dab5a4b5b7eb115f4fa8e6deffc1a160d20ec911d053595ca3afd5f6a</v>
       </c>
       <c r="B64">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C64">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D64">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>6c47e6a8cf60feac3b11097bbac7d181512fcbbc351af20c67ff823eb3378f7e</v>
+        <v>a56bfc9381bf4196b9de6651cfd24088f4e362acae2bd70c78eddb55fccf684d</v>
       </c>
       <c r="B65">
-        <v>1742457968682</v>
+        <v>1742469357505</v>
       </c>
       <c r="C65">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D65">
-        <v>2060</v>
+        <v>627</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>6ef13607d170acec1d1edb1b578ec8807399528d6fc36feeee18d4fc14a465b7</v>
+        <v>4b4ba4ea37c39634972feef2df754d78a1fe577e9e63135286dc35d52416baf9</v>
       </c>
       <c r="B66">
-        <v>1742457968682</v>
+        <v>1742469357506</v>
       </c>
       <c r="C66">
-        <v>1742457970742</v>
+        <v>1742469359741</v>
       </c>
       <c r="D66">
-        <v>2060</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>aec4c5f9b8823dee5265f2dd14dc24246dc60c26b2e3b5915bf4b73af52281cc</v>
+        <v>27c4299d30118589d91454194df928dc10d2bf06f6976c56bb9f07ff8032c7f8</v>
       </c>
       <c r="B67">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C67">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D67">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>e13d9be19539b52313dcb7e55fc8344f7e4cf291367d2d3cea366cb7e88f6e38</v>
+        <v>4949c0a07cb4b2e0354dada84a2dde2c9027e73a11070c1ea5d25dab795102c6</v>
       </c>
       <c r="B68">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C68">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D68">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>bb46eef24bea7a45dace49aaacfb7796065d48c9a8740ee9b9a7310950c9ab05</v>
+        <v>a0d23f8d565e9cdb7f498452e44b327ca367623b505bfa0eab59284e59be34a2</v>
       </c>
       <c r="B69">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C69">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D69">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>b5f31b0e7461b2365101a80970f1d8714d6e170e91619a1dd67961ad2807784d</v>
+        <v>5fa5c575c15263be73194b374a945ac956b57d2ff23d7a1085aa7f3906474759</v>
       </c>
       <c r="B70">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C70">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D70">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>0d241a28bfc1a879cd8569526e9c0c55663b1dab3e1a7a1923973997ea389ae4</v>
+        <v>56f90df2f8714bb9fdcb59893e26a639bd605350ff8364e6a0734e652e44ff7a</v>
       </c>
       <c r="B71">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C71">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D71">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>7042c481b34b3b150ac7a26eaf51ea152221dedbb8d16021f2f4c267052380db</v>
+        <v>f32b1ac3205e51db4e8fcc46a061a528ac1ef6121ff8eb8c8ec2ce02d83480bb</v>
       </c>
       <c r="B72">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C72">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D72">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>060f554244a113bf9df607a370199631fe6f8cbe67f9553da8eef68b73c86fff</v>
+        <v>f0f2a42b5fe6945545afb31248eea4eaaa5dc341744d92f21c74b4fbc66c84b4</v>
       </c>
       <c r="B73">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C73">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D73">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>2b492038774b806f88c6648951c52c94474bc4005ad87ce63e3c6f7151241919</v>
+        <v>ac9aec5c74aa0a61d46f70dd6de36e90a23628429085038692ff33960848c4b3</v>
       </c>
       <c r="B74">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C74">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D74">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>4237feb2287c4dd235dd8aa19d27c4c068c0721700bde8c2c2b905b1485eeaaa</v>
+        <v>1ca9ad6b8455902358d76b1fb7eef41ee940cbb987be312e7b483dcbca6d11e9</v>
       </c>
       <c r="B75">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C75">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D75">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>d40c3801456ef8074005416b953fc5dde46e1a4054ebadb37d36282cf0562cf4</v>
+        <v>a9bbb35d0c489627a0007ecfb63ef1c9a34dccde91a3f20dd2cb121ca9031f5d</v>
       </c>
       <c r="B76">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C76">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D76">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>e26bbf66644672fcf896df71d0c48fe276a01dba9e093480258f5b153f107bee</v>
+        <v>c4a861cd2be3a1b5ebcab6222777d0d9f79874d2a2245e0d6d93d7eb14227aae</v>
       </c>
       <c r="B77">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C77">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D77">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>0f3910b5ee818cc2e3197fdc103b61f0af5c64ba59096e4723f30c476aa3b42b</v>
+        <v>44dd94c5289c5279090ab7c02f55efcc50d955dd773161f3cc6fe260d104898c</v>
       </c>
       <c r="B78">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C78">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D78">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>c79e386e2cdf414056099dc71fdd546c5b4a86c8841bba990aa6714afe0486ae</v>
+        <v>f5071fa0abe0855e162f856c463d75d1fc700c8af032ca254ea3ea38c830142c</v>
       </c>
       <c r="B79">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C79">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D79">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>42384b8b1ea86405fe862016f929a4206db3f2c3ceba5ab1650929f755f42458</v>
+        <v>4bc34ee5bc527479dd255b1bf596f8f33559e68f78ecd574fa42a142df93833e</v>
       </c>
       <c r="B80">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C80">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D80">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>53110c180f5a5e8a106eab02d4eed868a6cb10be07c3ba582c53449ec3c0a0f9</v>
+        <v>d4620b54f61b2b3d5ca68203d4c78587d354caf525d84549c3e633766dde0e25</v>
       </c>
       <c r="B81">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C81">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D81">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>fcde8a5c2feb2c40b50ab6fb4fbf70163c966a0ac91837e5733437e8baa9e1b4</v>
+        <v>cd060a74474e926a3abc03789152c07b7b44943607eb08f6cdb691ef005bebb2</v>
       </c>
       <c r="B82">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C82">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D82">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>7602ea4ce6d6b14a55d2c72d70a3a7edf3685255ba76ba2196e6e0bbeda3ae12</v>
+        <v>23b54cf66b6eb174593c08f3e3f329b9ffa0e32a66f03ac9a0d75d03b7ace9c6</v>
       </c>
       <c r="B83">
-        <v>1742457968732</v>
+        <v>1742469357506</v>
       </c>
       <c r="C83">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D83">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>94dc831c95f04031f723ececc65674a1cc5d33a58ad1dbb818a95107925a6183</v>
+        <v>6bae94951ade7e063dc0e8b5d7c52477ce3597d1b458344fb338b42a74d263a1</v>
       </c>
       <c r="B84">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C84">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D84">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>960d297abb0303815c4f5ecb9ef3e263deb07ca25468a5a657f57733594b8382</v>
+        <v>8ce34e2c4bc704d3c0c26d0ef1fe549f203e5e94d175c7b160f8e88445a688ad</v>
       </c>
       <c r="B85">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C85">
-        <v>1742457971408</v>
+        <v>1742469359742</v>
       </c>
       <c r="D85">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>27877303008e786bfd6367e20c76c118ba09ae515ee0979d422c59360022b4e0</v>
+        <v>0c9ae9e917e1117f299ea204cf167850b6d4bc8cc66aa2e36f006dc6788e80b5</v>
       </c>
       <c r="B86">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C86">
-        <v>1742457971408</v>
+        <v>1742469359741</v>
       </c>
       <c r="D86">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>ad5877a8ff3e5bcadbc648e39e2b2b0006df2c51b3483b59290306a8fb06fc2f</v>
+        <v>8b259b8bd869050c2088419269b3bf2cb4f99068e5b245cccb5623aaa717f6b6</v>
       </c>
       <c r="B87">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C87">
-        <v>1742457971409</v>
+        <v>1742469359741</v>
       </c>
       <c r="D87">
-        <v>2677</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>be02346726d4ec1591012c22284b9a075fd1a26a78955c3aafaf5c8b0542ca93</v>
+        <v>eb0a3b148a10839f7c1783d41a0395cbfd454bb4e2284591656db83da0afe96d</v>
       </c>
       <c r="B88">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C88">
-        <v>1742457971408</v>
+        <v>1742469360785</v>
       </c>
       <c r="D88">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>afa881db28bfc231931aa046e69648a8cc5c115d8bb26163fd9eabf093b4098f</v>
+        <v>eb298a8ffc4efeb2a81f7fb0d020a0dec647a9dd92411f004c6599579078f892</v>
       </c>
       <c r="B89">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C89">
-        <v>1742457971408</v>
+        <v>1742469360785</v>
       </c>
       <c r="D89">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>da677c45f23322dd7dae84f8296e4ba8655aba74a156e9b82586ccee3e33b570</v>
+        <v>c7a6ccc879d1f7f542502629524d1a834566df1a4bf5558f4d1db9c3b3fa4b97</v>
       </c>
       <c r="B90">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C90">
-        <v>1742457971408</v>
+        <v>1742469359742</v>
       </c>
       <c r="D90">
-        <v>2676</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>07b801fb56d843b04ebeb72df3340b2e4f2fcf151574436fee56777dc7c981e6</v>
+        <v>4fcddc104bad2b024d733d61ac02fd64dbda61195501301d286a14538725018c</v>
       </c>
       <c r="B91">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C91">
-        <v>1742457971409</v>
+        <v>1742469359741</v>
       </c>
       <c r="D91">
-        <v>2676</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>ffafa5fd3d284734435c917b3d6f2ee95a68702d1d07ee0bfecf23d80fb38554</v>
+        <v>3cee136d702a64248c8648f355c015c1bcdbb0d24c19eb3f7698f6aa0ae02ec8</v>
       </c>
       <c r="B92">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C92">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D92">
-        <v>2677</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>679d0fdb54c6bfae61d45d28acba1289223299a703954e682640510e3d441fb0</v>
+        <v>a5c480bdc29e05eddc8a976d25f4da63f83a41b54ce9a6948f83d25929010536</v>
       </c>
       <c r="B93">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C93">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D93">
-        <v>2677</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>58fe0f1735724c6f55186f2f8ad41a596d6f03aeef2f7c8f2c2227f14f2be3b1</v>
+        <v>fc04cd327cacf589ca8f8156f6011fb4ea2e263e0eff82b480c614ce6336cf8d</v>
       </c>
       <c r="B94">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C94">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D94">
-        <v>2677</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>5173c86eda322f8850b4ef198c3f00dc24210b00530c67a4c66e7e07ca0e09b0</v>
+        <v>408712f37a8942dfe59f37e31b723a49b3b32d115af12b2bdaed5261e556b863</v>
       </c>
       <c r="B95">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C95">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D95">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>f388456afc4f31c95735536ea9947b4017bd2f6ac3b8c6b858209062d7f1b815</v>
+        <v>1b7092eef34e92f2bba8effb7871e959c06475ea3d7715751b226e8ff81f9484</v>
       </c>
       <c r="B96">
-        <v>1742457968732</v>
+        <v>1742469357507</v>
       </c>
       <c r="C96">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D96">
-        <v>2677</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>6a1e79996136b30ca469b23a4f691614728a946822615d12ba12120d5853123c</v>
+        <v>4f27ab3776c0bda4d90e01e8f8558ef6ebfdb32b61451b2b12f3d2c47cbce76e</v>
       </c>
       <c r="B97">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C97">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D97">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>453222832c2c94ea1d23f7fa97b73a6443ec34a13a4445b1b0406adb5504cfe6</v>
+        <v>4194124bfdbf42acab336376c106f4deb7d0ca9b5e8d30e96277914ef4ff63fb</v>
       </c>
       <c r="B98">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C98">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D98">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>07b646d0bc0426e01dfe0d868b2ad7f9d5b478dd917ad858ce08c531c721e25d</v>
+        <v>9d159f2befa42d40398b9a9407aa1f83a86501ae0f23d263bee81206e2dfb83f</v>
       </c>
       <c r="B99">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C99">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D99">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>1df70cf4b01c16c0d3a4d310c46820f64d36b9993a2722b0a10ecb3ec8d57a0f</v>
+        <v>12de265d3d0d21f3d10bf0aa0471579f1cff2ba2fd678dbcbf26859906d83389</v>
       </c>
       <c r="B100">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C100">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D100">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>6d6bfe5e287d5cf1fdc906f45fadcc12569b3ba4483cd4b3e5090fac18a59e3a</v>
+        <v>5b78488ca13898c5a0a9d8788614a3c0efc6e57cb51516061f05694c6be39b97</v>
       </c>
       <c r="B101">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C101">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D101">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>a52e954da7435f8c2c3360ba58a54fdac5deb59be1f4aad07f5eb4b10899f1b4</v>
+        <v>009546eb260019c86842447a6369b9930f20c427452b76b84b6b30a6f463c16c</v>
       </c>
       <c r="B102">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C102">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D102">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>0295a5f928cd1bdfce825aabe7f55c53ecdd5f88a0ed9b25761ffb6b5c89bdcc</v>
+        <v>bdbe326b43b517d65eb03117eddac4ac841fef89f15dccf22b4302b9e83e7739</v>
       </c>
       <c r="B103">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C103">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D103">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>3a8734e3cf290a69a1159bfd20e3f9ec992954d926e9b6a02d1da5bc45a01cf8</v>
+        <v>2849bebe826ab6ae9c5756ebcefe2fffbc3c00f583f9499c784215344b9e9131</v>
       </c>
       <c r="B104">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C104">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D104">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>288fdf337774695d13a8989af4fbdd24d16dd5b2f7e30d7d06eb7c4108cc52de</v>
+        <v>de2ca717fe09527142e989125831f89370a6a7473e754150cbe24d397815d33d</v>
       </c>
       <c r="B105">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C105">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D105">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>234e498ea2818a725096689b38b8aa781c9f9bd85b92ae575dd4273ecd1b0a96</v>
+        <v>f29cdd9dd590047ae929570f5c4fcac7ba48a5c7c3d8e84cbb47779f32fe7e42</v>
       </c>
       <c r="B106">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C106">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D106">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>d33a74b1f982417a17929ba2a22a2b0656ab10156993a7bae575ac1350bce7ff</v>
+        <v>378ff58d4b69d750b4d4224c419f4ca6a81228e8101970b311d8e91e660dffde</v>
       </c>
       <c r="B107">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C107">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D107">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>cca840c6302164feed5634c8ca303e63409cde255d3708492ab56e25df64e195</v>
+        <v>fd1c3830cfd3baa2dc19bf0a2d5f0a8f15ea318564a27f087d2c4dafeccb0440</v>
       </c>
       <c r="B108">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C108">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D108">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>00b46983f12b13bddae209c7b8a2a11eb56184aa7cae4758ed496de783501baf</v>
+        <v>6accb6b309958f2328fc3614bc52f4c50af95001862a41971a4ca9961fe2921c</v>
       </c>
       <c r="B109">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C109">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D109">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>e55ba8387f1b4d0ce1cf955ccc76d6b6fda9b3a151c7921f80a2a3cb5cd752b8</v>
+        <v>fb7be667109f55f3b2993a19d0cf2d9049783ccefc996cc1d83a1a0be2c58ebf</v>
       </c>
       <c r="B110">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C110">
-        <v>1742457971409</v>
+        <v>1742469360785</v>
       </c>
       <c r="D110">
-        <v>2676</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>7a9e989add6ed7a119dc9d80f7ba89b0f38825e549498baf5b309091cc9eea72</v>
+        <v>da929f63e40449a9622c350535a9b3d903be7fd03339b346df79d0f829a4c87a</v>
       </c>
       <c r="B111">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C111">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D111">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>6a0e55438d7d6e5611e6e3ead523eb4d68e9be5f29a20e49c1e65f9c59f55d4a</v>
+        <v>ef3cc0cf07c37ac1148359703e9bf1811edff7b3c782f761b151becb8cd010b9</v>
       </c>
       <c r="B112">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C112">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D112">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>72ddde1dff55dcd43de1c6e6de017520929c795a1cf9204b8bd47294850b4d3c</v>
+        <v>3aca0f61d15fc4c0ea5d0ed6a62a94279860734541d562dd0b8e51c781c34dd5</v>
       </c>
       <c r="B113">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C113">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D113">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>eeed71d9f483e94d2ea6c0c58541d8c489c36aef3f53e6d95fdd5c554ad37d37</v>
+        <v>946ea06b1281dfb9a1ea9e7dc0de6753839e8d570f44f6320b27875198715442</v>
       </c>
       <c r="B114">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C114">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D114">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>b1a90823485bbf774929ab13ce350d8ad0ad4a2d9f33f840f85a30212e6f48ba</v>
+        <v>f87e63b96ee0077108b9ce3fd80b43a6bbc11563f54934ff1cd8d91c69149cd6</v>
       </c>
       <c r="B115">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C115">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D115">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>8d9995cb9e2d41a5918f74637294ea27db75e36709fd93879c6ebfac0cab47c2</v>
+        <v>1729028ce85f55a9ec186f6edfa2147780be10ce9a1b4abb8e1fca62dd31fd94</v>
       </c>
       <c r="B116">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C116">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D116">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>05efc006d296d66495cd62aecc1f94e22dba4254aade4e61806a08785977b064</v>
+        <v>ad573365c4c438060ba0f230e863db0975c353327fb47940dc3695558671ea85</v>
       </c>
       <c r="B117">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C117">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D117">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>aab08f5e03adb4c2c3cdc02d57a5fb83d2bc7e46d502046335ed9247b2e75c7c</v>
+        <v>9fd4457403eeaaa0f0533a94374717b97d7b80dd798e5140ec93ee25900dc7bc</v>
       </c>
       <c r="B118">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C118">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D118">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>b32efca6c5851fb9099c896cfe3591afd15bb79064084b19e565f0f2bad9a4f6</v>
+        <v>928cb40ce636e7188988909bd41578fae329b3b507e6b67feb53a31c62a751d2</v>
       </c>
       <c r="B119">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C119">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D119">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>903f5ba38687a2c7a362cbc4158519e40b5ff89c1be2e131a57bfb5bb5cb10d3</v>
+        <v>06b56627bb42f11d451aea7616136ed602cee60ef91f7c5fc199d5caea0bf1dd</v>
       </c>
       <c r="B120">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C120">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D120">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>efc4faed1fafa1e5d1951cfc0a60c4b89d0394dee368e82fa6adc94b064a1ead</v>
+        <v>0026513a012640c47e49574d35b76b3de428d78939ef42f8c9c4ae5dc6e1d84f</v>
       </c>
       <c r="B121">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C121">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D121">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>37a5538eec0608e54ef8c3b9f24ba9ff6b5fa2c6a0cd1ac2f24dd5225df1fa22</v>
+        <v>cbb0bb3a1e9b7fffb6395d76aae38c8bb98816f1de8eefeac3860cc2e4c34e4f</v>
       </c>
       <c r="B122">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C122">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D122">
-        <v>2671</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>88d61445ff256f227413ed25bed11b9cb45963293ca2753d5144c11ff4421749</v>
+        <v>38ef0888c6dc69d3142bb154954b98339effdd503706d5361c8e57cf953135c4</v>
       </c>
       <c r="B123">
-        <v>1742457968733</v>
+        <v>1742469357507</v>
       </c>
       <c r="C123">
-        <v>1742457971404</v>
+        <v>1742469360785</v>
       </c>
       <c r="D123">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>9eb9a36b8f3b7310c3625cbcdb48d371f6d55185552d0006097b02967cefaec6</v>
+        <v>7a1d2c6014e095c38b86da147304ad44ab372af66ddb4f5833c314bd90ddee86</v>
       </c>
       <c r="B124">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C124">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D124">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>4ca7fc4ea5eb615583f026e97d1b09e4c2029573f56e5cdddf6f1d1fc1efa248</v>
+        <v>ad3560a9806215d293a342d9ff01e2c948f9fecab65599f40b730a626b935cbf</v>
       </c>
       <c r="B125">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C125">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D125">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>0124b265a1a299864c8dea19cc7a982eeba4ec6de5632ca091513d0a9c83bc51</v>
+        <v>505c72dd45c7fda61c940f40924902767c29effb546ce0933fbd25891862b800</v>
       </c>
       <c r="B126">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C126">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D126">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>97195d523da8ef573a4fca15778d2460d4a487ecb5c02595fd556872c1decf19</v>
+        <v>21f0e51c1894deeba0dec644e18a30116797db6dac4abce38040ae3a1057b099</v>
       </c>
       <c r="B127">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C127">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D127">
-        <v>2671</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>718b5b0a1cdc1962f04940a2b98e702218b08df388df41f56e47938756abe31c</v>
+        <v>4b54013c89cbd9f20f4b886aad623a469f4324c919c706a2dcde8fab7cd25abe</v>
       </c>
       <c r="B128">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C128">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D128">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>4e5f0bf4e21ab8fe9f2d09c0c2afaff92ec627592a5bddf451e55b0b451334ea</v>
+        <v>4968f71a7aed95ecb34fa0f4787ee8825b1e33a520e274e8c832cd5d91468853</v>
       </c>
       <c r="B129">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C129">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D129">
-        <v>2671</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>5b6eaec1f59c4531a03cec20436021ccc06fca3d085fee777ccf3fcb2d18bf3e</v>
+        <v>85e1034cdbfc1d93cd2c834d4ba97be990c43ded796265a6cca5a90df6652335</v>
       </c>
       <c r="B130">
-        <v>1742457968733</v>
+        <v>1742469357508</v>
       </c>
       <c r="C130">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D130">
-        <v>2671</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>1bcda396564d7d48c5201462ab9c73a1f1d7319b71b56c4edf144bb576374438</v>
+        <v>5b5e3bee301434d2b852df7aee6f395692757b44cfed8f393bbd144791c2037c</v>
       </c>
       <c r="B131">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C131">
-        <v>1742457971404</v>
+        <v>1742469360786</v>
       </c>
       <c r="D131">
-        <v>2670</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>d6fc84d694a44f609e8a1dd04f9be745336d3e0fe0698ef5c27de7a0c5722b05</v>
+        <v>3473a14c879de78e51020d790ab92acd44172a7f7019c6b26525fa977db7a76d</v>
       </c>
       <c r="B132">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C132">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D132">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>1c0a322b6bd53bd4d8bab66a14291f9922d509a0f2647610e2fcd335177a6eeb</v>
+        <v>a346c00fe650d5a6c44ecc3833f07e11f56671207ce817b1dea1d8dc176f3ade</v>
       </c>
       <c r="B133">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C133">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D133">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>f4e558b975a5795b56537bb5870b53f9e5b40f88726d050743f77082ad7f7aa3</v>
+        <v>6df5bec3010a9f7ab8f8c6fd554eaf2dd71cf007c39123e77280246dee69c00e</v>
       </c>
       <c r="B134">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C134">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D134">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>dd03180cb17111be41e2b5d81e039ea25dd24ebee89af31fa525c54b05c925dd</v>
+        <v>aa8141978a38726e8f30fa998448be1863751236ee2af394c7eb927a6426ba5c</v>
       </c>
       <c r="B135">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C135">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D135">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>0b03508c93762eecc52953cd746f56721a326afd16c4524e593be68e348e820f</v>
+        <v>133c10a7073e53d6aa8b7eba8495c4ea30ce2e79139b1f64fb618c664a41e045</v>
       </c>
       <c r="B136">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C136">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D136">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>68a3937c2ff2779b6761fc913e0c90bd75f38b72053516911fdbf09e1dc21999</v>
+        <v>7e4c83133e5b5aedc322aaed705fc4860d1afbe29d9de6a8c466c8af48b994fd</v>
       </c>
       <c r="B137">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C137">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D137">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>4830f742b9c33cab1e535c0f872b3ddca10fde4bb1047b2eddc65c0002157f06</v>
+        <v>b627dbdee6b361fa8da6321191e643d611e1249ba2792377c52dbcc69af4a920</v>
       </c>
       <c r="B138">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C138">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D138">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>2cca9746c7cf917f8bada8e05de35de87b9181e03c6f04438d7516e64ab3d775</v>
+        <v>ea5e0004d0da716baf7fea2dbc476bb854b83e3b3814edaa1ccc910545cdeb15</v>
       </c>
       <c r="B139">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C139">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D139">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>e73451dd2f47ce00b363931b7fc0331990e92ec89577efd7788083cbc4673e9f</v>
+        <v>ad3e4cfd774ac0392d25b0c9dec999d26da0a15dcf892cda02f74d6f7839a420</v>
       </c>
       <c r="B140">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C140">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D140">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>bca45172331f68993e7e329f6eb2511ffb5fa3dc32836173f66d937b5372747f</v>
+        <v>950870b94fe9061322c0f696fa7eb7f62eab8818e8e124801d5c8953951b3f7d</v>
       </c>
       <c r="B141">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C141">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D141">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>0e01e50c36db2dd0f661225b515a2878ee9db15ed64d4b39b938cefccfed8f08</v>
+        <v>ca5f7515ceee200139c4536a71441681532b83f106830085c9b8710aecc40b05</v>
       </c>
       <c r="B142">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C142">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D142">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>f5ce6fcf6110b4b3266d7174ddd2374c29855b3d4ed00cfb91c3f663f6fce1c4</v>
+        <v>53fdebc1792e9c72074418ddd9edbf966c1e86c5df9930e41a4411983be935a9</v>
       </c>
       <c r="B143">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C143">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D143">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>7a697ef3bd6f2f89e65355dd84c6165b1ceb488d3e0c0dd1d57d9ffbd1195c4d</v>
+        <v>2a64e192762440b2614b74489442be93e5cb6b6d7cedaea664a2677961ff2858</v>
       </c>
       <c r="B144">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C144">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D144">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>f413137554920a05a2467f6c490db2974ab4e9ad7431d54b393b744ce75e0645</v>
+        <v>83af73c3691f6649a7c5dbd288f5241146e3bb2dee9c9795943ffdbdf43573c9</v>
       </c>
       <c r="B145">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C145">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D145">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>e1744b8c5e6f26cd5d665a764fa3e76972ceaa0c038b27f99fd10e223980879f</v>
+        <v>4e04225e2734d159afcde6c94aea93404323ac13598560656fca8d332cc590eb</v>
       </c>
       <c r="B146">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C146">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D146">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>35996c3869fd09f8bdb181669e5cfb83b7840b3ed4bb370e7b983842f5e8b8b4</v>
+        <v>19ce86472d5c16095fc597ecd8408488b0a30c175a9c9029ad9f6892845d4e9e</v>
       </c>
       <c r="B147">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C147">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D147">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>2e9518f282506c6f3071516cbdc08867c39e9bbaac312dd124a8367bae7cdccc</v>
+        <v>a10c29be01dc3eb9791947df55303a975c329abfdd0a49e3eba1153fa88c16c8</v>
       </c>
       <c r="B148">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C148">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D148">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>65dbd3a57d8f696b0ceaf5df763b990779c1178a6a10f101d5811d18944028e3</v>
+        <v>092d65b2b33c13d553a8754d21ba1fddb669600301bcaefac3fa7840dc493598</v>
       </c>
       <c r="B149">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C149">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D149">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>76b87c13e538f14445d257e210ec060e264bc1e34e79a2909fd0147e22c7b507</v>
+        <v>1bb3303a9bb51415c6711e8a637efd3e8cf7789ce9be46d213bc0ea3300a5ff7</v>
       </c>
       <c r="B150">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C150">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D150">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>2be7dcce4d74e20d2510157c9a4900cfa7b6a91795128fc1f7ce7ef6eac3fffb</v>
+        <v>14d50dc7431ca500fdb0e759bc893ff4a689da68276f33621b8f4808a0103b43</v>
       </c>
       <c r="B151">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C151">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D151">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>4a2777c64a94072add16890b2378eda9e2b3501b6b6658a5ee38d9dee91f4ca8</v>
+        <v>66de4a3f146160378b444f1a819db7633ce5da25acd69926bc896d351dbd5090</v>
       </c>
       <c r="B152">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C152">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D152">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>a18db104225f250595afc16dde76bb8ca2524d13ba7071af446a38ee9c987e9c</v>
+        <v>3d53c1d44b599140ae1f9b400858fd2da02e5b2d95ee4951708cf46229faf053</v>
       </c>
       <c r="B153">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C153">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D153">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>8b6a74cedf943ea9a6c652055c1bd10d58d582f7d31123c44d867b9b9332f412</v>
+        <v>69e0b7afd8e2765b54fd8fe29ef928fb25402f7fc6db5a654014538a88591b4b</v>
       </c>
       <c r="B154">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C154">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D154">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>443a9acc326c95d02aa9afc7dcca83d50a17b2b49c0179a4005ad9b846b9e3ec</v>
+        <v>a8c58f0e9996fc2f7e08ac5dc7dffc5b9ddb290c65e117770514d15162f61afe</v>
       </c>
       <c r="B155">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C155">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D155">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>cbaa01935b9a69f117961bfb3f474b408625b50a2b19f7cf1336fe36762b687c</v>
+        <v>26dd33aaa67dc20a5c7773dd7a98a076b85b663612cbcc835a4e97fd59032f97</v>
       </c>
       <c r="B156">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C156">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D156">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>440773ee1566aecb1a1d99fc01244815a1f401242f83a8f6b60f9ca12bab40ff</v>
+        <v>2e37e97571317445a998315759a7c4d8a84a29bd153e337567c171f6d23d82dd</v>
       </c>
       <c r="B157">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C157">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D157">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>7f3adecc7cf510098429d82c8cd7efeb234b087459c6846e2223221203d5ee10</v>
+        <v>d176b67729203b1b5d6fb6f893fe6f93a0eeaca4cb62d27f9cf00ea677007dd7</v>
       </c>
       <c r="B158">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C158">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D158">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>97492deff91fe68b054b9e68fd35e27484f5c8a10016a11233971c754e1bfb6e</v>
+        <v>aa3e9e8744524b6f919a610e7af1fa6d8474a12ba7b87350430c50f2b7cbe398</v>
       </c>
       <c r="B159">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C159">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D159">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>0101c7ec2251924d000cffe3ec56a0c3c816cda6c6c4ec58aff39802ff53c3ee</v>
+        <v>97b3bdd9335b932610553b3e35e331779170d757934d1c3216d7bbc0494fd789</v>
       </c>
       <c r="B160">
-        <v>1742457968983</v>
+        <v>1742469357508</v>
       </c>
       <c r="C160">
-        <v>1742457970742</v>
+        <v>1742469360787</v>
       </c>
       <c r="D160">
-        <v>1759</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>9a5afb8e2dbd19580241d93fb2d023ba9bcedc35e561124d6434b803266b58c0</v>
+        <v>88d312ac09558894b648980e19b8f2d38b3f44744228e9dc18186dbff2a00471</v>
       </c>
       <c r="B161">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C161">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D161">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>47cd5c7004a381d5b677ee1e3853d145b77ce6c604341c8d206e79cc38764c96</v>
+        <v>20f3414b8925176e64433e6a45a11890d5043639b7859ea2f277829296d921e8</v>
       </c>
       <c r="B162">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C162">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D162">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>7173560f387f1a3b5b8d7bc77c60a4a33ce8dcab23696ffb53673372d69df83d</v>
+        <v>cf1b92a7a8b903f9e6f67b4ffdc46aba69a1f3164eb89baba077889e00713a08</v>
       </c>
       <c r="B163">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C163">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D163">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>04e2a60c298189c81f029f3d892a1446a8548fc387eb56da13f7ad6cfa651279</v>
+        <v>ae6f038793d1e73bacff300feddd171d6f6d4533b93191cf90c15a40a75194ea</v>
       </c>
       <c r="B164">
-        <v>1742457968984</v>
+        <v>1742469357508</v>
       </c>
       <c r="C164">
-        <v>1742457970742</v>
+        <v>1742469360788</v>
       </c>
       <c r="D164">
-        <v>1758</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>d1c2a75e90fac65f0bcc9f6d7e343a9cb650cf878f4987ef93a9df4c22487175</v>
+        <v>4262363373e610bfaa228d14fafc505c57377ecf1c851dcc79468da22376c397</v>
       </c>
       <c r="B165">
-        <v>1742457968734</v>
+        <v>1742469357805</v>
       </c>
       <c r="C165">
-        <v>1742457971404</v>
+        <v>1742469358132</v>
       </c>
       <c r="D165">
-        <v>2670</v>
+        <v>327</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
-        <v>e4087536de79a85689aac9352de95a69bd5db10feb13581cce445aafef18cf21</v>
+        <v>1ec701fafdd8ca62e3c5ebc94e20a0c58f82d5e0b8cb9d446d79ebce78eb43cf</v>
       </c>
       <c r="B166">
-        <v>1742457968734</v>
+        <v>1742469357508</v>
       </c>
       <c r="C166">
-        <v>1742457971404</v>
+        <v>1742469360787</v>
       </c>
       <c r="D166">
-        <v>2670</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>e098321b496f86f04d635386e15d7f84425400cc2ca2c884da898fbddbc823a0</v>
+        <v>f2521039101836491de860ee3f873de04a5781a8b6812f805166002d1599b3aa</v>
       </c>
       <c r="B167">
-        <v>1742457968984</v>
+        <v>1742469357508</v>
       </c>
       <c r="C167">
-        <v>1742457970742</v>
+        <v>1742469360787</v>
       </c>
       <c r="D167">
-        <v>1758</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
-        <v>3e6f93d3d5c8fc6f60d576e928463c9e37389bce0b0c043b35e0fcd4e83b29dc</v>
+        <v>78771d74b3f40adb2c71582b517858b43d4d3c22915987f808a0f56f3ccc6780</v>
       </c>
       <c r="B168">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C168">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D168">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>764e9b1d7ec9303dddbd717f735a7a32c1d04a0e8a133e43e38f75fcd6e69b5c</v>
+        <v>1706fbb4ae895f22d29e8bed29cba105a5fcbec12b45012f5741302e8fb512bf</v>
       </c>
       <c r="B169">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C169">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D169">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>7907aca1ee9f4a25712408fea2e8c6ef1c53046bb053326a0113177be734afdb</v>
+        <v>c3bc27b60a2c69f33baebb3040fda697a6d08306a83ddb8902af3991b5d64027</v>
       </c>
       <c r="B170">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C170">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D170">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>21f0e6f193b7716f620e5a47868c05557787d646db47d1858bd4c468b5944bb8</v>
+        <v>98a6653d1a7852fc913b11557895dca4aaccd74f9fc22d92425ea4e57765b7d2</v>
       </c>
       <c r="B171">
-        <v>1742457968984</v>
+        <v>1742469357508</v>
       </c>
       <c r="C171">
-        <v>1742457970742</v>
+        <v>1742469360788</v>
       </c>
       <c r="D171">
-        <v>1758</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
-        <v>d7922ced2bca65cf5d8ae8360fc254a0fba46a74ff08d751010185900af96aa1</v>
+        <v>27864f95d78a1b758fbe6663dea7a3453b5c958d714875b8f85b8d0d41ea208a</v>
       </c>
       <c r="B172">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C172">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D172">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
-        <v>4c782e2b69f143f6cd67880060a4e261ae37a7139c792f6dadfaf88831836ae7</v>
+        <v>d13fefdd1f724aac3a32ff505f595ad15a3a6acdf709c3723af38d90219293e3</v>
       </c>
       <c r="B173">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C173">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D173">
-        <v>1758</v>
+        <v>328</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>22f37726f3296b397debec4e22293a3cfe6df7eecf6e7cb62ceb721972a03021</v>
+        <v>62984cc7ea001b57acb475bf955b67b256521b58c0f587563a8da245698dd7ba</v>
       </c>
       <c r="B174">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C174">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D174">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
-        <v>a7b71cf067cafdad98a2da1cafee52119f6b6247875f409ad3786a70ab5ef510</v>
+        <v>280d7f33c1086218687a8669d735cdd0740c54c3095d4f39bf884a2ec70c4bdf</v>
       </c>
       <c r="B175">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C175">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D175">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
-        <v>5d3e0cc66c06bd387c233f5f68be8e6b49901562c3007cd626399fa45321f019</v>
+        <v>2a554442011d5e431f4ee8434033bc663d17051b6bed97b1e3febdc912d72efb</v>
       </c>
       <c r="B176">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C176">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D176">
-        <v>1758</v>
+        <v>328</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>2656f4b0492c76bcbf3cbba76a4249841bb11d6db9e6ac7766f03351d27f9c18</v>
+        <v>81b708980433a03cba4429159bab38ae6a87297da56e4696f86ad8621a2bcf3d</v>
       </c>
       <c r="B177">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C177">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D177">
-        <v>1758</v>
+        <v>328</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>20829f43c455645819f1b4ba702cb7d1bd0b2edb57416ac9b96049d250316b39</v>
+        <v>64eb8bc93e25719678cc96dbe17c5635927d9d402e7b8be5f658ec8e75f00072</v>
       </c>
       <c r="B178">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C178">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D178">
-        <v>1758</v>
+        <v>328</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>ef7ae5111cc1380b2bf591dd01486bd035f26618999770f8b30571f4dfcb2cac</v>
+        <v>539724277b24c788843b807e9fabee2ad49a7433fea31c3a2690bb5c3b1d18d1</v>
       </c>
       <c r="B179">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C179">
-        <v>1742457970742</v>
+        <v>1742469358132</v>
       </c>
       <c r="D179">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>29256a3ca8f26f73d7f2d4ade36b824290381bcfa6a366b6e914b01ae1ba4b38</v>
+        <v>540425faa8ca567276f18ba8b5258bf785f23f330d020583be75a3d3c2f4f67b</v>
       </c>
       <c r="B180">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C180">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D180">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>1709082435d679f7ba1c94ddffc0e6e315326b994dc2316202ad3f6b0f685341</v>
+        <v>7eddf01cd9e2bffce6da3639e9fd0f20612f33eaf866019a087eab6a6901c89a</v>
       </c>
       <c r="B181">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C181">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D181">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>2bf6766fea0a08b5b9bee0548d40db6ab927b724fb462e6e59ae7b176dc61aaf</v>
+        <v>4540f97a108fa28ad8d84d7ba89d7b7bd21d310224a368832e08ed8a5f57534b</v>
       </c>
       <c r="B182">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C182">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D182">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>12b7ecff4dc146af162182424a30724fb9b65764b9796ef29e41bf0861a4f6d3</v>
+        <v>5af1c727804c4233df3beaa1bcb0ffc8e2419fed40a11e5f88ac1f1de71831c4</v>
       </c>
       <c r="B183">
-        <v>1742457968984</v>
+        <v>1742469357805</v>
       </c>
       <c r="C183">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D183">
-        <v>1758</v>
+        <v>328</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>a79b019e2f410feeacbe333fa0526a4dc2389c9d00564d14e3447ab826152c1b</v>
+        <v>0a02d5b7d1769ad5b020f603dd006478781f3278c6e06977db6569375765f102</v>
       </c>
       <c r="B184">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C184">
-        <v>1742457970742</v>
+        <v>1742469358340</v>
       </c>
       <c r="D184">
-        <v>1758</v>
+        <v>534</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>dff057cd593e0cce12381b478a76058d80747a7c44366222b91b459a6bb59b03</v>
+        <v>42568ef8a11b5bd93cfe5b68cb5d3f60c36b5293e2e628c2a426f540d42d9ef8</v>
       </c>
       <c r="B185">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C185">
-        <v>1742457970742</v>
+        <v>1742469358340</v>
       </c>
       <c r="D185">
-        <v>1758</v>
+        <v>534</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>96530b6040d31d8ab2f92d28f75ef36fa6d6a36e83cba8bbfa9f48e29600e8d1</v>
+        <v>3688c2796c2f147084982b7bdd476ad62dfc13bf00664302afacb73f392c6462</v>
       </c>
       <c r="B186">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C186">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D186">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>fad26ad9ffefd79cbb0e6bfee9154e82c61aa19b12bac62de28c7a7f5c4fe562</v>
+        <v>cec561c4d254022d3b1d6d7b9468ab819df06dcba725d3567b0832a621fea3a6</v>
       </c>
       <c r="B187">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C187">
-        <v>1742457970742</v>
+        <v>1742469358133</v>
       </c>
       <c r="D187">
-        <v>1758</v>
+        <v>327</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>e27b7cafa48dcf32a10923b0321c98c195eedf730857f45f1c2f876568dc321e</v>
+        <v>10aff4d525047bc7e78b1c41057b898be785145374ae8f530569364aa24b507d</v>
       </c>
       <c r="B188">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C188">
-        <v>1742457970742</v>
+        <v>1742469358341</v>
       </c>
       <c r="D188">
-        <v>1758</v>
+        <v>535</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
-        <v>512e37aec881d43feb60ad6c1e20690dce0c3dbe8f1ce0b00953f37b735fe415</v>
+        <v>94dcfd41fb171f30d84427fb0a1771cdbc3507dd0dc69ab3fb19370dcbfbbd77</v>
       </c>
       <c r="B189">
-        <v>1742457968984</v>
+        <v>1742469357806</v>
       </c>
       <c r="C189">
-        <v>1742457970742</v>
+        <v>1742469358341</v>
       </c>
       <c r="D189">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="str">
-        <v>b5cbc303af268627051fae38eaddfd34a0ee454a79cd6cf1c6d85715cf69002f</v>
-      </c>
-      <c r="B190">
-        <v>1742457968984</v>
-      </c>
-      <c r="C190">
-        <v>1742457970742</v>
-      </c>
-      <c r="D190">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="str">
-        <v>99e0f27aa9940a9c4f349d257a0a0e5501354c66a720011d2462096276d8539f</v>
-      </c>
-      <c r="B191">
-        <v>1742457968985</v>
-      </c>
-      <c r="C191">
-        <v>1742457970742</v>
-      </c>
-      <c r="D191">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="str">
-        <v>947001203ec202c1249f5dfac30740029e37e0fc35b0b6f8e4498ee2005eb391</v>
-      </c>
-      <c r="B192">
-        <v>1742457968984</v>
-      </c>
-      <c r="C192">
-        <v>1742457970742</v>
-      </c>
-      <c r="D192">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="str">
-        <v>e594af5574051b915afb07b5e02df4f898f7fad46bfb0339d39fd6f2d08d1d03</v>
-      </c>
-      <c r="B193">
-        <v>1742457968984</v>
-      </c>
-      <c r="C193">
-        <v>1742457970742</v>
-      </c>
-      <c r="D193">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="str">
-        <v>cf6716c1a3d24e7dc03162725dacf862b3a90e94f674b1e3c2d2de2df1602391</v>
-      </c>
-      <c r="B194">
-        <v>1742457968984</v>
-      </c>
-      <c r="C194">
-        <v>1742457970742</v>
-      </c>
-      <c r="D194">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="str">
-        <v>07f04764029427e9040536fc7a1e547aef44e6d49cace5fbe89416ecdde8c023</v>
-      </c>
-      <c r="B195">
-        <v>1742457968985</v>
-      </c>
-      <c r="C195">
-        <v>1742457970742</v>
-      </c>
-      <c r="D195">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="str">
-        <v>71df57b510f19a040248cd16d1b89b7749fa4ef8d856e458b0f193eda268c702</v>
-      </c>
-      <c r="B196">
-        <v>1742457968985</v>
-      </c>
-      <c r="C196">
-        <v>1742457970742</v>
-      </c>
-      <c r="D196">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="str">
-        <v>b6e37380f1d42e54714db52d2e588e1d2f9d2f46170fa9cc67b7d93f28fec2b9</v>
-      </c>
-      <c r="B197">
-        <v>1742457968985</v>
-      </c>
-      <c r="C197">
-        <v>1742457970742</v>
-      </c>
-      <c r="D197">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="str">
-        <v>d345dfa369e34eb65c26f3cdf2f759800eef00639d9c441dce2bac5d7c6d7105</v>
-      </c>
-      <c r="B198">
-        <v>1742457968985</v>
-      </c>
-      <c r="C198">
-        <v>1742457970742</v>
-      </c>
-      <c r="D198">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="str">
-        <v>ef5db2ffea783b45541f2ef2d19a76ec709ff75c1a3d337914d1984f0b8957c1</v>
-      </c>
-      <c r="B199">
-        <v>1742457968985</v>
-      </c>
-      <c r="C199">
-        <v>1742457970743</v>
-      </c>
-      <c r="D199">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="str">
-        <v>b8fb390ea009b76848cf22372e1a0b3ff4919b3f70df5572eb81214c7432db29</v>
-      </c>
-      <c r="B200">
-        <v>1742457968985</v>
-      </c>
-      <c r="C200">
-        <v>1742457970742</v>
-      </c>
-      <c r="D200">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="str">
-        <v>8a6e23897ac0dcf266739c3548b1bbdb3ab14542110478ea2ea22042bd8fa562</v>
-      </c>
-      <c r="B201">
-        <v>1742457968985</v>
-      </c>
-      <c r="C201">
-        <v>1742457970742</v>
-      </c>
-      <c r="D201">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="str">
-        <v>ae7552751ef40935808943fd41f7dbb2c1ac625d0402e33898ac71dc73886ba0</v>
-      </c>
-      <c r="B202">
-        <v>1742457968985</v>
-      </c>
-      <c r="C202">
-        <v>1742457970742</v>
-      </c>
-      <c r="D202">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="str">
-        <v>722bd4e61358ccf05703455e707035c1b2952e3e59c91a0c44e191f2f763238e</v>
-      </c>
-      <c r="B203">
-        <v>1742457969293</v>
-      </c>
-      <c r="C203">
-        <v>1742457969875</v>
-      </c>
-      <c r="D203">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="str">
-        <v>2a1158ccd2d2ae01d7279aecfcf023a69046a1fdecab483310da7b387cd11752</v>
-      </c>
-      <c r="B204">
-        <v>1742457969293</v>
-      </c>
-      <c r="C204">
-        <v>1742457969875</v>
-      </c>
-      <c r="D204">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="str">
-        <v>4cfbffcc7afc1d00472d9b12dc39bc2c4a253b026393c08c8fe94e09b51e9839</v>
-      </c>
-      <c r="B205">
-        <v>1742457969293</v>
-      </c>
-      <c r="C205">
-        <v>1742457969875</v>
-      </c>
-      <c r="D205">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="str">
-        <v>9b7943d8128cd65a4712d6a46e5b534a702f36ba9e1886ff0c55022b6ad7705c</v>
-      </c>
-      <c r="B206">
-        <v>1742457969293</v>
-      </c>
-      <c r="C206">
-        <v>1742457969875</v>
-      </c>
-      <c r="D206">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="str">
-        <v>00ffa145b4c14b0a873be3b43ca594b440da547a10b3c7b324c8fc1ee25425af</v>
-      </c>
-      <c r="B207">
-        <v>1742457969293</v>
-      </c>
-      <c r="C207">
-        <v>1742457969875</v>
-      </c>
-      <c r="D207">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="str">
-        <v>5d6ad510b2828c0623402071a035095344121471c5c664c645011b774b71ccdc</v>
-      </c>
-      <c r="B208">
-        <v>1742457969293</v>
-      </c>
-      <c r="C208">
-        <v>1742457969875</v>
-      </c>
-      <c r="D208">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="str">
-        <v>57c8d2f3582456d426507a95f217214bfc0a7427072afafaff17b067522c3d60</v>
-      </c>
-      <c r="B209">
-        <v>1742457969293</v>
-      </c>
-      <c r="C209">
-        <v>1742457969875</v>
-      </c>
-      <c r="D209">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="str">
-        <v>586480a23b574dc2212c881fdf15903472806817a75614bdb91d0a0544e354f0</v>
-      </c>
-      <c r="B210">
-        <v>1742457969293</v>
-      </c>
-      <c r="C210">
-        <v>1742457969875</v>
-      </c>
-      <c r="D210">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="str">
-        <v>e85c59b7a2cf196fbab5c23c71876320d14f1e18fa40eed5667984cb2fad2aa2</v>
-      </c>
-      <c r="B211">
-        <v>1742457969293</v>
-      </c>
-      <c r="C211">
-        <v>1742457969876</v>
-      </c>
-      <c r="D211">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="str">
-        <v>a3375b07443dae8f06ba539129f6eec293ae320ab53c0e914c3d7d8416eba7e8</v>
-      </c>
-      <c r="B212">
-        <v>1742457969293</v>
-      </c>
-      <c r="C212">
-        <v>1742457969875</v>
-      </c>
-      <c r="D212">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="str">
-        <v>3a67985d9ff0f72c8d0baf4a19e49910e34a33886c7393bdcd8f921ddfecd4e7</v>
-      </c>
-      <c r="B213">
-        <v>1742457969293</v>
-      </c>
-      <c r="C213">
-        <v>1742457969875</v>
-      </c>
-      <c r="D213">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="str">
-        <v>2529bfe8202d76a16f6564b264dafd6f6ee5446f280652c4071da4337811962c</v>
-      </c>
-      <c r="B214">
-        <v>1742457969293</v>
-      </c>
-      <c r="C214">
-        <v>1742457969875</v>
-      </c>
-      <c r="D214">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="str">
-        <v>70d8436fd46179b649cc75f8d538e6b0eb3673b1e8cfc21a32c4f221dd1dac2f</v>
-      </c>
-      <c r="B215">
-        <v>1742457969293</v>
-      </c>
-      <c r="C215">
-        <v>1742457969876</v>
-      </c>
-      <c r="D215">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="str">
-        <v>439f25b4b6cb9f51ee820058896a471e7ef654b95a7731455f7c42f5c3553db5</v>
-      </c>
-      <c r="B216">
-        <v>1742457969293</v>
-      </c>
-      <c r="C216">
-        <v>1742457969875</v>
-      </c>
-      <c r="D216">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="str">
-        <v>1c2dd485cdf9f6f1cfaa4563a0d23a825c3464930050c90071305d6979c55c24</v>
-      </c>
-      <c r="B217">
-        <v>1742457969293</v>
-      </c>
-      <c r="C217">
-        <v>1742457969876</v>
-      </c>
-      <c r="D217">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="str">
-        <v>fe334529d58d72545d7db1edcbc5c3f64ccc169fac62a68c325bc86fa21d6610</v>
-      </c>
-      <c r="B218">
-        <v>1742457969293</v>
-      </c>
-      <c r="C218">
-        <v>1742457969876</v>
-      </c>
-      <c r="D218">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="str">
-        <v>a02b8090010c505fc36c736306061438d3328a25d239f08ff787ad0485ec49f5</v>
-      </c>
-      <c r="B219">
-        <v>1742457969294</v>
-      </c>
-      <c r="C219">
-        <v>1742457969876</v>
-      </c>
-      <c r="D219">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="str">
-        <v>641989e28459c236e4978b367cb8401e8696c13356fdd096caa95906b4f0ba95</v>
-      </c>
-      <c r="B220">
-        <v>1742457969293</v>
-      </c>
-      <c r="C220">
-        <v>1742457969876</v>
-      </c>
-      <c r="D220">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="str">
-        <v>4287a3f4d5ccf52ece7a35240ccc4fee0c5c86c81f9ff519596a4c52feb92022</v>
-      </c>
-      <c r="B221">
-        <v>1742457969293</v>
-      </c>
-      <c r="C221">
-        <v>1742457969876</v>
-      </c>
-      <c r="D221">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="str">
-        <v>dd74bac17e2217d9534af4298e81bfba82de593da7ef8abfc8eac6365a9e5f1a</v>
-      </c>
-      <c r="B222">
-        <v>1742457969293</v>
-      </c>
-      <c r="C222">
-        <v>1742457969876</v>
-      </c>
-      <c r="D222">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="str">
-        <v>5e2bd54dd491762d8d4c543449773c348e23a5786d00e420c85607e805d5c19d</v>
-      </c>
-      <c r="B223">
-        <v>1742457969294</v>
-      </c>
-      <c r="C223">
-        <v>1742457969876</v>
-      </c>
-      <c r="D223">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="str">
-        <v>54e2603680d4506bf8077e054cf1de6e0a3495fb6b00df91ffe99efd494d9ff8</v>
-      </c>
-      <c r="B224">
-        <v>1742457969294</v>
-      </c>
-      <c r="C224">
-        <v>1742457969876</v>
-      </c>
-      <c r="D224">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="str">
-        <v>734f5ac8698738f2f7851c3e830fb320602edd274578b520a20edf0d504a9eba</v>
-      </c>
-      <c r="B225">
-        <v>1742457969294</v>
-      </c>
-      <c r="C225">
-        <v>1742457969876</v>
-      </c>
-      <c r="D225">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="str">
-        <v>ac85ae0d5f7801048891264eb6113a9f312a85a6704400c4afcffd86b5a05f7f</v>
-      </c>
-      <c r="B226">
-        <v>1742457969294</v>
-      </c>
-      <c r="C226">
-        <v>1742457969876</v>
-      </c>
-      <c r="D226">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="str">
-        <v>395c206c97fc1f134f8b7c1202461ba2297f91d30111119f0a89c2afd63dec28</v>
-      </c>
-      <c r="B227">
-        <v>1742457969294</v>
-      </c>
-      <c r="C227">
-        <v>1742457969876</v>
-      </c>
-      <c r="D227">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="str">
-        <v>6e9ef93943fca9a31dda0c259767ded59b8e93a2957bfde134c617426763a886</v>
-      </c>
-      <c r="B228">
-        <v>1742457969294</v>
-      </c>
-      <c r="C228">
-        <v>1742457969876</v>
-      </c>
-      <c r="D228">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="str">
-        <v>5b86a1a73880c69ede8905239e0452585fc37c51a45ee5ae504ff8feeb3958d6</v>
-      </c>
-      <c r="B229">
-        <v>1742457969294</v>
-      </c>
-      <c r="C229">
-        <v>1742457969876</v>
-      </c>
-      <c r="D229">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="str">
-        <v>bef6ab9f7af5798fa9e8c1b24f79b30c877a06fb08dc7b664bd7d3c5b07709ee</v>
-      </c>
-      <c r="B230">
-        <v>1742457969294</v>
-      </c>
-      <c r="C230">
-        <v>1742457969876</v>
-      </c>
-      <c r="D230">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="str">
-        <v>9d881d2afd5b22a5c45d9a153ce4f9c3179238655e66a72f50c5a7e078c826af</v>
-      </c>
-      <c r="B231">
-        <v>1742457969294</v>
-      </c>
-      <c r="C231">
-        <v>1742457969876</v>
-      </c>
-      <c r="D231">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="str">
-        <v>3e3f53da50b49fd8d0726b0bbf0734dad32311ce1e44311d2c99e1c60871e8db</v>
-      </c>
-      <c r="B232">
-        <v>1742457969294</v>
-      </c>
-      <c r="C232">
-        <v>1742457969876</v>
-      </c>
-      <c r="D232">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="str">
-        <v>ab1bdf9f1fbb247c3d23967cc4021c29ffa0e61718fd7c00ff0b0d1304be0f4c</v>
-      </c>
-      <c r="B233">
-        <v>1742457969294</v>
-      </c>
-      <c r="C233">
-        <v>1742457969876</v>
-      </c>
-      <c r="D233">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="str">
-        <v>005de8393a22fe5c18a22ca430a27b463936252a56202663b807bc6286e5d6ae</v>
-      </c>
-      <c r="B234">
-        <v>1742457969294</v>
-      </c>
-      <c r="C234">
-        <v>1742457969876</v>
-      </c>
-      <c r="D234">
-        <v>582</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D234"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D189"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>